<commit_message>
add rating_data for all agencies
</commit_message>
<xml_diff>
--- a/files/ratings.xlsx
+++ b/files/ratings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="845">
   <si>
     <t xml:space="preserve">Belgium </t>
   </si>
@@ -2029,61 +2029,64 @@
     <t xml:space="preserve">Oct 05 2010</t>
   </si>
   <si>
+    <t xml:space="preserve">C-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar 02 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 09 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 23 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 17 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 26 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apr 27 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 23 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oct 05 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sep 27 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 27 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 19 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 03 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 06 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar 24 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov 06 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oct 23 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aug 24 2010</t>
+  </si>
+  <si>
     <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mar 02 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 09 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feb 23 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 17 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan 26 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apr 27 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 23 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oct 05 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sep 27 1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feb 27 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan 19 2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feb 03 1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 06 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mar 24 2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nov 06 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oct 23 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aug 24 2010</t>
   </si>
   <si>
     <t xml:space="preserve">Feb 22 2012</t>
@@ -2945,11 +2948,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U45" activeCellId="0" sqref="U45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.25"/>
@@ -2960,17 +2963,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="29" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="68" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="71" style="0" width="8.67"/>
@@ -11146,7 +11149,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E45" s="11" t="s">
         <v>56</v>
       </c>
@@ -11380,10 +11383,10 @@
         <v>29</v>
       </c>
       <c r="U47" s="12" t="s">
-        <v>669</v>
+        <v>688</v>
       </c>
       <c r="V47" s="14" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="W47" s="11" t="s">
         <v>32</v>
@@ -11392,7 +11395,7 @@
         <v>52</v>
       </c>
       <c r="Y47" s="14" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="AF47" s="11" t="s">
         <v>29</v>
@@ -11419,7 +11422,7 @@
         <v>108</v>
       </c>
       <c r="AN47" s="14" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="AR47" s="11" t="s">
         <v>29</v>
@@ -11437,7 +11440,7 @@
         <v>35</v>
       </c>
       <c r="BI47" s="14" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="BJ47" s="11" t="s">
         <v>32</v>
@@ -11446,7 +11449,7 @@
         <v>117</v>
       </c>
       <c r="BL47" s="13" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="BM47" s="11" t="s">
         <v>56</v>
@@ -11455,7 +11458,7 @@
         <v>65</v>
       </c>
       <c r="BO47" s="14" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="BP47" s="11" t="s">
         <v>32</v>
@@ -11464,7 +11467,7 @@
         <v>46</v>
       </c>
       <c r="BR47" s="14" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11475,7 +11478,7 @@
         <v>44</v>
       </c>
       <c r="S48" s="13" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="T48" s="11" t="s">
         <v>32</v>
@@ -11484,7 +11487,7 @@
         <v>291</v>
       </c>
       <c r="V48" s="14" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="W48" s="11" t="s">
         <v>32</v>
@@ -11502,7 +11505,7 @@
         <v>44</v>
       </c>
       <c r="AH48" s="14" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="AI48" s="11" t="s">
         <v>29</v>
@@ -11511,7 +11514,7 @@
         <v>74</v>
       </c>
       <c r="AK48" s="14" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="AL48" s="11" t="s">
         <v>32</v>
@@ -11520,7 +11523,7 @@
         <v>48</v>
       </c>
       <c r="AN48" s="14" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="AR48" s="11" t="s">
         <v>56</v>
@@ -11529,7 +11532,7 @@
         <v>187</v>
       </c>
       <c r="AT48" s="14" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="BG48" s="11" t="s">
         <v>56</v>
@@ -11538,7 +11541,7 @@
         <v>69</v>
       </c>
       <c r="BI48" s="14" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="BJ48" s="11" t="s">
         <v>29</v>
@@ -11547,7 +11550,7 @@
         <v>482</v>
       </c>
       <c r="BL48" s="13" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="BM48" s="11" t="s">
         <v>29</v>
@@ -11556,7 +11559,7 @@
         <v>59</v>
       </c>
       <c r="BO48" s="14" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="BP48" s="11" t="s">
         <v>32</v>
@@ -11565,7 +11568,7 @@
         <v>33</v>
       </c>
       <c r="BR48" s="14" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11582,10 +11585,10 @@
         <v>56</v>
       </c>
       <c r="U49" s="12" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="V49" s="14" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="W49" s="11" t="s">
         <v>29</v>
@@ -11594,7 +11597,7 @@
         <v>52</v>
       </c>
       <c r="Y49" s="14" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="AF49" s="11" t="s">
         <v>56</v>
@@ -11603,7 +11606,7 @@
         <v>133</v>
       </c>
       <c r="AH49" s="14" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="AI49" s="11" t="s">
         <v>56</v>
@@ -11621,7 +11624,7 @@
         <v>33</v>
       </c>
       <c r="AN49" s="14" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AR49" s="11" t="s">
         <v>32</v>
@@ -11630,7 +11633,7 @@
         <v>42</v>
       </c>
       <c r="AT49" s="14" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="BG49" s="11" t="s">
         <v>29</v>
@@ -11639,7 +11642,7 @@
         <v>44</v>
       </c>
       <c r="BI49" s="14" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="BJ49" s="11" t="s">
         <v>56</v>
@@ -11648,7 +11651,7 @@
         <v>547</v>
       </c>
       <c r="BL49" s="13" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="BM49" s="11" t="s">
         <v>56</v>
@@ -11657,7 +11660,7 @@
         <v>65</v>
       </c>
       <c r="BO49" s="14" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="BP49" s="11" t="s">
         <v>56</v>
@@ -11666,7 +11669,7 @@
         <v>108</v>
       </c>
       <c r="BR49" s="14" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11677,7 +11680,7 @@
         <v>44</v>
       </c>
       <c r="S50" s="13" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="T50" s="11" t="s">
         <v>29</v>
@@ -11686,7 +11689,7 @@
         <v>236</v>
       </c>
       <c r="V50" s="14" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="W50" s="11" t="s">
         <v>32</v>
@@ -11695,7 +11698,7 @@
         <v>67</v>
       </c>
       <c r="Y50" s="14" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="AF50" s="11" t="s">
         <v>56</v>
@@ -11704,7 +11707,7 @@
         <v>133</v>
       </c>
       <c r="AH50" s="14" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="AI50" s="11" t="s">
         <v>32</v>
@@ -11713,7 +11716,7 @@
         <v>74</v>
       </c>
       <c r="AK50" s="14" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="AL50" s="11" t="s">
         <v>29</v>
@@ -11722,7 +11725,7 @@
         <v>33</v>
       </c>
       <c r="AN50" s="14" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="AR50" s="11" t="s">
         <v>29</v>
@@ -11740,7 +11743,7 @@
         <v>35</v>
       </c>
       <c r="BI50" s="14" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="BJ50" s="11" t="s">
         <v>56</v>
@@ -11749,7 +11752,7 @@
         <v>334</v>
       </c>
       <c r="BL50" s="13" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="BM50" s="11" t="s">
         <v>29</v>
@@ -11767,7 +11770,7 @@
         <v>61</v>
       </c>
       <c r="BR50" s="14" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11778,7 +11781,7 @@
         <v>57</v>
       </c>
       <c r="S51" s="13" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="T51" s="11" t="s">
         <v>32</v>
@@ -11787,7 +11790,7 @@
         <v>236</v>
       </c>
       <c r="V51" s="14" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="W51" s="11" t="s">
         <v>56</v>
@@ -11796,7 +11799,7 @@
         <v>71</v>
       </c>
       <c r="Y51" s="14" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="AF51" s="11" t="s">
         <v>32</v>
@@ -11805,7 +11808,7 @@
         <v>67</v>
       </c>
       <c r="AH51" s="14" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="AI51" s="11" t="s">
         <v>32</v>
@@ -11814,7 +11817,7 @@
         <v>48</v>
       </c>
       <c r="AK51" s="14" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="AL51" s="11" t="s">
         <v>29</v>
@@ -11832,7 +11835,7 @@
         <v>95</v>
       </c>
       <c r="AT51" s="14" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="BG51" s="11" t="s">
         <v>32</v>
@@ -11850,7 +11853,7 @@
         <v>569</v>
       </c>
       <c r="BL51" s="13" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="BM51" s="11" t="s">
         <v>56</v>
@@ -11859,7 +11862,7 @@
         <v>95</v>
       </c>
       <c r="BO51" s="14" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="BP51" s="11" t="s">
         <v>29</v>
@@ -11868,7 +11871,7 @@
         <v>33</v>
       </c>
       <c r="BR51" s="14" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11879,7 +11882,7 @@
         <v>44</v>
       </c>
       <c r="S52" s="13" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="T52" s="11" t="s">
         <v>56</v>
@@ -11888,7 +11891,7 @@
         <v>450</v>
       </c>
       <c r="V52" s="14" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="W52" s="11" t="s">
         <v>56</v>
@@ -11897,7 +11900,7 @@
         <v>69</v>
       </c>
       <c r="Y52" s="14" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="AF52" s="11" t="s">
         <v>56</v>
@@ -11906,7 +11909,7 @@
         <v>57</v>
       </c>
       <c r="AH52" s="14" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="AI52" s="11" t="s">
         <v>29</v>
@@ -11915,7 +11918,7 @@
         <v>48</v>
       </c>
       <c r="AK52" s="14" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="AL52" s="11" t="s">
         <v>56</v>
@@ -11924,7 +11927,7 @@
         <v>108</v>
       </c>
       <c r="AN52" s="14" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="AR52" s="11" t="s">
         <v>29</v>
@@ -11942,7 +11945,7 @@
         <v>44</v>
       </c>
       <c r="BI52" s="14" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="BJ52" s="11" t="s">
         <v>32</v>
@@ -11951,7 +11954,7 @@
         <v>482</v>
       </c>
       <c r="BL52" s="13" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="BM52" s="11" t="s">
         <v>29</v>
@@ -11960,7 +11963,7 @@
         <v>59</v>
       </c>
       <c r="BO52" s="14" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="BP52" s="11" t="s">
         <v>32</v>
@@ -11969,7 +11972,7 @@
         <v>33</v>
       </c>
       <c r="BR52" s="14" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11980,7 +11983,7 @@
         <v>71</v>
       </c>
       <c r="S53" s="13" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="T53" s="11" t="s">
         <v>29</v>
@@ -12007,7 +12010,7 @@
         <v>67</v>
       </c>
       <c r="AH53" s="14" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="AI53" s="11" t="s">
         <v>29</v>
@@ -12025,7 +12028,7 @@
         <v>33</v>
       </c>
       <c r="AN53" s="14" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="AR53" s="11" t="s">
         <v>56</v>
@@ -12034,7 +12037,7 @@
         <v>63</v>
       </c>
       <c r="AT53" s="14" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="BG53" s="11" t="s">
         <v>29</v>
@@ -12052,7 +12055,7 @@
         <v>482</v>
       </c>
       <c r="BL53" s="13" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="BM53" s="11" t="s">
         <v>56</v>
@@ -12061,7 +12064,7 @@
         <v>95</v>
       </c>
       <c r="BO53" s="14" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="BP53" s="11" t="s">
         <v>56</v>
@@ -12070,7 +12073,7 @@
         <v>61</v>
       </c>
       <c r="BR53" s="14" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12090,7 +12093,7 @@
         <v>547</v>
       </c>
       <c r="V54" s="14" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="W54" s="11" t="s">
         <v>29</v>
@@ -12117,7 +12120,7 @@
         <v>48</v>
       </c>
       <c r="AK54" s="14" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="AL54" s="11" t="s">
         <v>29</v>
@@ -12126,7 +12129,7 @@
         <v>46</v>
       </c>
       <c r="AN54" s="14" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="AR54" s="11" t="s">
         <v>56</v>
@@ -12135,7 +12138,7 @@
         <v>63</v>
       </c>
       <c r="AT54" s="14" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="BG54" s="11" t="s">
         <v>32</v>
@@ -12144,7 +12147,7 @@
         <v>30</v>
       </c>
       <c r="BI54" s="14" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="BJ54" s="11" t="s">
         <v>56</v>
@@ -12153,7 +12156,7 @@
         <v>334</v>
       </c>
       <c r="BL54" s="13" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="BM54" s="11" t="s">
         <v>29</v>
@@ -12162,7 +12165,7 @@
         <v>42</v>
       </c>
       <c r="BO54" s="14" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="BP54" s="11" t="s">
         <v>32</v>
@@ -12171,7 +12174,7 @@
         <v>46</v>
       </c>
       <c r="BR54" s="14" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12191,7 +12194,7 @@
         <v>40</v>
       </c>
       <c r="V55" s="14" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="W55" s="11" t="s">
         <v>32</v>
@@ -12200,7 +12203,7 @@
         <v>67</v>
       </c>
       <c r="Y55" s="14" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="AF55" s="11" t="s">
         <v>32</v>
@@ -12209,7 +12212,7 @@
         <v>67</v>
       </c>
       <c r="AH55" s="14" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="AI55" s="11" t="s">
         <v>56</v>
@@ -12218,7 +12221,7 @@
         <v>121</v>
       </c>
       <c r="AK55" s="14" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="AL55" s="21" t="s">
         <v>56</v>
@@ -12227,7 +12230,7 @@
         <v>99</v>
       </c>
       <c r="AN55" s="24" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="AR55" s="11" t="s">
         <v>32</v>
@@ -12236,7 +12239,7 @@
         <v>74</v>
       </c>
       <c r="AT55" s="14" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="BG55" s="11" t="s">
         <v>32</v>
@@ -12245,7 +12248,7 @@
         <v>44</v>
       </c>
       <c r="BI55" s="14" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="BJ55" s="21" t="s">
         <v>29</v>
@@ -12254,7 +12257,7 @@
         <v>482</v>
       </c>
       <c r="BL55" s="23" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="BM55" s="11" t="s">
         <v>32</v>
@@ -12263,7 +12266,7 @@
         <v>59</v>
       </c>
       <c r="BO55" s="14" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="BP55" s="21" t="s">
         <v>32</v>
@@ -12272,7 +12275,7 @@
         <v>482</v>
       </c>
       <c r="BR55" s="24" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12283,7 +12286,7 @@
         <v>52</v>
       </c>
       <c r="S56" s="13" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="T56" s="11" t="s">
         <v>32</v>
@@ -12310,7 +12313,7 @@
         <v>71</v>
       </c>
       <c r="AH56" s="24" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="AI56" s="21" t="s">
         <v>32</v>
@@ -12319,7 +12322,7 @@
         <v>48</v>
       </c>
       <c r="AK56" s="24" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="AR56" s="11" t="s">
         <v>29</v>
@@ -12328,7 +12331,7 @@
         <v>74</v>
       </c>
       <c r="AT56" s="14" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="BG56" s="11" t="s">
         <v>29</v>
@@ -12346,7 +12349,7 @@
         <v>95</v>
       </c>
       <c r="BO56" s="24" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12357,7 +12360,7 @@
         <v>71</v>
       </c>
       <c r="S57" s="13" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="T57" s="11" t="s">
         <v>56</v>
@@ -12366,7 +12369,7 @@
         <v>547</v>
       </c>
       <c r="V57" s="14" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="W57" s="11" t="s">
         <v>32</v>
@@ -12375,7 +12378,7 @@
         <v>44</v>
       </c>
       <c r="Y57" s="14" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AR57" s="11" t="s">
         <v>56</v>
@@ -12384,7 +12387,7 @@
         <v>63</v>
       </c>
       <c r="AT57" s="14" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="BG57" s="11" t="s">
         <v>32</v>
@@ -12393,7 +12396,7 @@
         <v>44</v>
       </c>
       <c r="BI57" s="14" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12404,7 +12407,7 @@
         <v>52</v>
       </c>
       <c r="S58" s="13" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="T58" s="11" t="s">
         <v>29</v>
@@ -12413,7 +12416,7 @@
         <v>46</v>
       </c>
       <c r="V58" s="14" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="W58" s="11" t="s">
         <v>29</v>
@@ -12431,7 +12434,7 @@
         <v>48</v>
       </c>
       <c r="AT58" s="14" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="BG58" s="11" t="s">
         <v>29</v>
@@ -12451,7 +12454,7 @@
         <v>52</v>
       </c>
       <c r="S59" s="13" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="T59" s="11" t="s">
         <v>29</v>
@@ -12478,7 +12481,7 @@
         <v>121</v>
       </c>
       <c r="AT59" s="14" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="BG59" s="11" t="s">
         <v>56</v>
@@ -12507,7 +12510,7 @@
         <v>108</v>
       </c>
       <c r="V60" s="14" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="W60" s="11" t="s">
         <v>32</v>
@@ -12516,7 +12519,7 @@
         <v>44</v>
       </c>
       <c r="Y60" s="14" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="AR60" s="11" t="s">
         <v>56</v>
@@ -12525,7 +12528,7 @@
         <v>61</v>
       </c>
       <c r="AT60" s="14" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="BG60" s="11" t="s">
         <v>32</v>
@@ -12534,7 +12537,7 @@
         <v>30</v>
       </c>
       <c r="BI60" s="14" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12554,7 +12557,7 @@
         <v>46</v>
       </c>
       <c r="V61" s="14" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="W61" s="21" t="s">
         <v>56</v>
@@ -12563,7 +12566,7 @@
         <v>69</v>
       </c>
       <c r="Y61" s="24" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="AR61" s="11" t="s">
         <v>32</v>
@@ -12581,7 +12584,7 @@
         <v>133</v>
       </c>
       <c r="BI61" s="14" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12601,7 +12604,7 @@
         <v>108</v>
       </c>
       <c r="V62" s="14" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="AR62" s="11" t="s">
         <v>56</v>
@@ -12610,7 +12613,7 @@
         <v>61</v>
       </c>
       <c r="AT62" s="14" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="BG62" s="11" t="s">
         <v>29</v>
@@ -12648,7 +12651,7 @@
         <v>48</v>
       </c>
       <c r="AT63" s="14" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="BG63" s="11" t="s">
         <v>32</v>
@@ -12657,7 +12660,7 @@
         <v>30</v>
       </c>
       <c r="BI63" s="14" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12677,7 +12680,7 @@
         <v>95</v>
       </c>
       <c r="V64" s="14" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="AR64" s="11" t="s">
         <v>29</v>
@@ -12686,7 +12689,7 @@
         <v>33</v>
       </c>
       <c r="AT64" s="14" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="BG64" s="11" t="s">
         <v>32</v>
@@ -12695,7 +12698,7 @@
         <v>35</v>
       </c>
       <c r="BI64" s="14" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12706,7 +12709,7 @@
         <v>57</v>
       </c>
       <c r="S65" s="13" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="T65" s="11" t="s">
         <v>56</v>
@@ -12715,7 +12718,7 @@
         <v>95</v>
       </c>
       <c r="V65" s="14" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="AR65" s="11" t="s">
         <v>56</v>
@@ -12724,7 +12727,7 @@
         <v>61</v>
       </c>
       <c r="AT65" s="14" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="BG65" s="11" t="s">
         <v>32</v>
@@ -12733,7 +12736,7 @@
         <v>59</v>
       </c>
       <c r="BI65" s="14" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12744,7 +12747,7 @@
         <v>57</v>
       </c>
       <c r="S66" s="13" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="T66" s="11" t="s">
         <v>29</v>
@@ -12753,7 +12756,7 @@
         <v>33</v>
       </c>
       <c r="V66" s="14" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="AR66" s="11" t="s">
         <v>32</v>
@@ -12762,7 +12765,7 @@
         <v>33</v>
       </c>
       <c r="AT66" s="14" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="BG66" s="11" t="s">
         <v>32</v>
@@ -12782,7 +12785,7 @@
         <v>69</v>
       </c>
       <c r="S67" s="13" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="T67" s="11" t="s">
         <v>32</v>
@@ -12791,7 +12794,7 @@
         <v>74</v>
       </c>
       <c r="V67" s="14" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="AR67" s="11" t="s">
         <v>56</v>
@@ -12800,7 +12803,7 @@
         <v>108</v>
       </c>
       <c r="AT67" s="14" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="BG67" s="11" t="s">
         <v>32</v>
@@ -12809,7 +12812,7 @@
         <v>59</v>
       </c>
       <c r="BI67" s="14" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12820,7 +12823,7 @@
         <v>44</v>
       </c>
       <c r="S68" s="13" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="T68" s="11" t="s">
         <v>56</v>
@@ -12829,7 +12832,7 @@
         <v>65</v>
       </c>
       <c r="V68" s="14" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="AR68" s="11" t="s">
         <v>29</v>
@@ -12838,7 +12841,7 @@
         <v>33</v>
       </c>
       <c r="AT68" s="14" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="BG68" s="21" t="s">
         <v>56</v>
@@ -12847,7 +12850,7 @@
         <v>187</v>
       </c>
       <c r="BI68" s="24" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12858,7 +12861,7 @@
         <v>67</v>
       </c>
       <c r="S69" s="13" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="T69" s="11" t="s">
         <v>32</v>
@@ -12867,7 +12870,7 @@
         <v>74</v>
       </c>
       <c r="V69" s="14" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="AR69" s="11" t="s">
         <v>32</v>
@@ -12876,7 +12879,7 @@
         <v>46</v>
       </c>
       <c r="AT69" s="14" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12887,7 +12890,7 @@
         <v>69</v>
       </c>
       <c r="S70" s="13" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="T70" s="11" t="s">
         <v>29</v>
@@ -12896,7 +12899,7 @@
         <v>74</v>
       </c>
       <c r="V70" s="14" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="AR70" s="11" t="s">
         <v>32</v>
@@ -12905,7 +12908,7 @@
         <v>46</v>
       </c>
       <c r="AT70" s="14" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12916,7 +12919,7 @@
         <v>133</v>
       </c>
       <c r="S71" s="13" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="T71" s="11" t="s">
         <v>32</v>
@@ -12925,7 +12928,7 @@
         <v>42</v>
       </c>
       <c r="V71" s="14" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="AR71" s="11" t="s">
         <v>32</v>
@@ -12934,7 +12937,7 @@
         <v>46</v>
       </c>
       <c r="AT71" s="14" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12945,7 +12948,7 @@
         <v>30</v>
       </c>
       <c r="S72" s="13" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="T72" s="11" t="s">
         <v>56</v>
@@ -12954,7 +12957,7 @@
         <v>187</v>
       </c>
       <c r="V72" s="14" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="AR72" s="11" t="s">
         <v>32</v>
@@ -12963,7 +12966,7 @@
         <v>46</v>
       </c>
       <c r="AT72" s="14" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12974,7 +12977,7 @@
         <v>30</v>
       </c>
       <c r="S73" s="13" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="T73" s="11" t="s">
         <v>29</v>
@@ -12983,7 +12986,7 @@
         <v>42</v>
       </c>
       <c r="V73" s="14" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="AR73" s="11" t="s">
         <v>56</v>
@@ -12992,7 +12995,7 @@
         <v>108</v>
       </c>
       <c r="AT73" s="14" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13012,7 +13015,7 @@
         <v>59</v>
       </c>
       <c r="V74" s="14" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="AR74" s="21" t="s">
         <v>56</v>
@@ -13021,7 +13024,7 @@
         <v>121</v>
       </c>
       <c r="AT74" s="24" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13032,7 +13035,7 @@
         <v>35</v>
       </c>
       <c r="S75" s="13" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="T75" s="11" t="s">
         <v>56</v>
@@ -13041,7 +13044,7 @@
         <v>187</v>
       </c>
       <c r="V75" s="14" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13052,7 +13055,7 @@
         <v>133</v>
       </c>
       <c r="S76" s="23" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="T76" s="11" t="s">
         <v>32</v>
@@ -13061,7 +13064,7 @@
         <v>42</v>
       </c>
       <c r="V76" s="14" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13072,7 +13075,7 @@
         <v>59</v>
       </c>
       <c r="V77" s="14" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13083,7 +13086,7 @@
         <v>59</v>
       </c>
       <c r="V78" s="14" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13094,7 +13097,7 @@
         <v>59</v>
       </c>
       <c r="V79" s="14" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13105,7 +13108,7 @@
         <v>187</v>
       </c>
       <c r="V80" s="14" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13116,7 +13119,7 @@
         <v>59</v>
       </c>
       <c r="V81" s="14" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13138,7 +13141,7 @@
         <v>35</v>
       </c>
       <c r="V83" s="14" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13149,7 +13152,7 @@
         <v>35</v>
       </c>
       <c r="V84" s="14" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13160,7 +13163,7 @@
         <v>35</v>
       </c>
       <c r="V85" s="14" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13171,7 +13174,7 @@
         <v>35</v>
       </c>
       <c r="V86" s="14" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13182,7 +13185,7 @@
         <v>187</v>
       </c>
       <c r="V87" s="14" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13204,7 +13207,7 @@
         <v>59</v>
       </c>
       <c r="V89" s="14" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13215,7 +13218,7 @@
         <v>59</v>
       </c>
       <c r="V90" s="14" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13237,7 +13240,7 @@
         <v>42</v>
       </c>
       <c r="V92" s="14" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13248,7 +13251,7 @@
         <v>74</v>
       </c>
       <c r="V93" s="14" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13259,7 +13262,7 @@
         <v>42</v>
       </c>
       <c r="V94" s="14" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13270,7 +13273,7 @@
         <v>74</v>
       </c>
       <c r="V95" s="14" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13281,7 +13284,7 @@
         <v>48</v>
       </c>
       <c r="V96" s="14" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13292,7 +13295,7 @@
         <v>65</v>
       </c>
       <c r="V97" s="14" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13314,7 +13317,7 @@
         <v>48</v>
       </c>
       <c r="V99" s="14" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13325,7 +13328,7 @@
         <v>63</v>
       </c>
       <c r="V100" s="14" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13336,7 +13339,7 @@
         <v>48</v>
       </c>
       <c r="V101" s="14" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13347,7 +13350,7 @@
         <v>33</v>
       </c>
       <c r="V102" s="24" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>